<commit_message>
Failsafe pulse generator adapted for different requirements of WS2813B-V5, Schematic reannotated, Footprint in WS2813 variant fixed
</commit_message>
<xml_diff>
--- a/HW/measurements/2024-01-17_TLC555 oscillator.xlsx
+++ b/HW/measurements/2024-01-17_TLC555 oscillator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\fsch\night-cones\HW\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F174D66D-487F-4376-BEFE-DCCADE62521E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728F64BF-E775-44F5-B13F-8B17B13AB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="17325" xr2:uid="{B453192C-7FC5-4FA6-9910-8EB9AAF63ADD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{B453192C-7FC5-4FA6-9910-8EB9AAF63ADD}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -406,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C81BE18-1CBC-403E-80BA-3F12BCF1F729}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1.0000000000000001E-9</v>
       </c>
@@ -453,11 +453,8 @@
       <c r="F2">
         <v>2478</v>
       </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -477,7 +474,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -497,7 +494,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -517,7 +514,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -537,7 +534,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -557,7 +554,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4.7000000000000003E-10</v>
       </c>
@@ -575,6 +572,206 @@
       </c>
       <c r="F8">
         <v>1424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9">
+        <v>1315</v>
+      </c>
+      <c r="E9">
+        <v>641.70000000000005</v>
+      </c>
+      <c r="F9">
+        <v>1957</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B10">
+        <v>1500</v>
+      </c>
+      <c r="C10">
+        <v>1500</v>
+      </c>
+      <c r="D10">
+        <v>1479</v>
+      </c>
+      <c r="E10">
+        <v>857.4</v>
+      </c>
+      <c r="F10">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B11">
+        <v>1500</v>
+      </c>
+      <c r="C11">
+        <v>1300</v>
+      </c>
+      <c r="D11">
+        <v>1406</v>
+      </c>
+      <c r="E11">
+        <v>768</v>
+      </c>
+      <c r="F11">
+        <v>2174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+      <c r="C12">
+        <v>1300</v>
+      </c>
+      <c r="D12">
+        <v>1190</v>
+      </c>
+      <c r="E12">
+        <v>787.8</v>
+      </c>
+      <c r="F12">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B13">
+        <v>910</v>
+      </c>
+      <c r="C13">
+        <v>1300</v>
+      </c>
+      <c r="D13">
+        <v>1155</v>
+      </c>
+      <c r="E13">
+        <v>794.4</v>
+      </c>
+      <c r="F13">
+        <v>1949</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B14">
+        <v>680</v>
+      </c>
+      <c r="C14">
+        <v>1300</v>
+      </c>
+      <c r="D14">
+        <v>1050</v>
+      </c>
+      <c r="E14">
+        <v>821</v>
+      </c>
+      <c r="F14">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>470</v>
+      </c>
+      <c r="B15">
+        <v>680</v>
+      </c>
+      <c r="C15">
+        <v>1200</v>
+      </c>
+      <c r="D15">
+        <v>1004</v>
+      </c>
+      <c r="E15">
+        <v>767</v>
+      </c>
+      <c r="F15">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B16">
+        <v>750</v>
+      </c>
+      <c r="C16">
+        <v>1200</v>
+      </c>
+      <c r="D16">
+        <v>1053</v>
+      </c>
+      <c r="E16">
+        <v>776.3</v>
+      </c>
+      <c r="F16">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B17">
+        <v>820</v>
+      </c>
+      <c r="C17">
+        <v>1200</v>
+      </c>
+      <c r="D17">
+        <v>1070</v>
+      </c>
+      <c r="E17">
+        <v>762.1</v>
+      </c>
+      <c r="F17">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B18">
+        <v>910</v>
+      </c>
+      <c r="C18">
+        <v>1200</v>
+      </c>
+      <c r="D18">
+        <v>1130</v>
+      </c>
+      <c r="E18">
+        <v>771.2</v>
+      </c>
+      <c r="F18">
+        <v>1901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HW: Failsafe oscillator measurements continued
</commit_message>
<xml_diff>
--- a/HW/measurements/2024-01-17_TLC555 oscillator.xlsx
+++ b/HW/measurements/2024-01-17_TLC555 oscillator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Daniel\fsch\night-cones\HW\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728F64BF-E775-44F5-B13F-8B17B13AB95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119D9520-AF3A-4299-8329-038E569E8992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17325" xr2:uid="{B453192C-7FC5-4FA6-9910-8EB9AAF63ADD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>C</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>t_l</t>
+  </si>
+  <si>
+    <t>NC1-1AA - 007</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C81BE18-1CBC-403E-80BA-3F12BCF1F729}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +777,51 @@
         <v>1901</v>
       </c>
     </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4.7000000000000003E-10</v>
+      </c>
+      <c r="B21">
+        <v>1500</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>1257</v>
+      </c>
+      <c r="E21">
+        <v>433</v>
+      </c>
+      <c r="F21">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2.1999999999999999E-10</v>
+      </c>
+      <c r="B22">
+        <v>1500</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>771</v>
+      </c>
+      <c r="E22">
+        <v>410</v>
+      </c>
+      <c r="F22">
+        <v>1186</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>